<commit_message>
Insert sorted excel data into DB
</commit_message>
<xml_diff>
--- a/HullMaintenance/Documents/SmartHull_Dev_Imabari(230119, 백업, Import용).xlsx
+++ b/HullMaintenance/Documents/SmartHull_Dev_Imabari(230119, 백업, Import용).xlsx
@@ -624,7 +624,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1901" uniqueCount="641">
   <si>
     <t>No</t>
   </si>
@@ -3871,11 +3871,6 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>Spis의 BHN File의 형상이 연결되지 않는 것으로 출력됨.
-실제 형상은 문제가 없음</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>010_Spec(Incl. FBack)\20230111\20230111_SmartHull_Feedback_CompareBHN.xlsx</t>
   </si>
   <si>
@@ -3970,6 +3965,30 @@
   <si>
     <t>Part List 작성 시 부재 수량이 다르게 출력되는 문제
 Assembly 설정이 잘못되어 발생한 문제</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>이마바리</t>
+  </si>
+  <si>
+    <t>이지철</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Spis의 BHN File의 형상이 연결되지 않는 것으로 출력됨.
+실제 형상은 문제가 없음
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">   - 소수점 문제는 미해결하였지만 같은 오차값으로 비교하여 비교시 에러는 나지 않도록 수정</t>
+    </r>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -4233,7 +4252,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4426,9 +4445,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -4437,6 +4453,24 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6511,10 +6545,10 @@
   <dimension ref="A1:S217"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="6" topLeftCell="H7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C223" sqref="C223"/>
+      <selection pane="bottomRight" activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.8984375" defaultRowHeight="24.9" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -6808,7 +6842,7 @@
         <v>568</v>
       </c>
       <c r="M9" s="35" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="N9" s="33" t="s">
         <v>619</v>
@@ -6900,17 +6934,17 @@
         <v>61</v>
       </c>
       <c r="M11" s="35" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="N11" s="33"/>
       <c r="O11" s="37" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="P11" s="35" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="Q11" s="40" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="R11" s="38"/>
       <c r="S11" s="39"/>
@@ -6938,20 +6972,20 @@
       </c>
       <c r="K12" s="36"/>
       <c r="L12" s="35" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="M12" s="35" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="N12" s="33"/>
       <c r="O12" s="37" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="P12" s="35" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="Q12" s="40" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="R12" s="38"/>
       <c r="S12" s="39"/>
@@ -6979,25 +7013,25 @@
       </c>
       <c r="K13" s="36"/>
       <c r="L13" s="35" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="M13" s="35" t="s">
         <v>210</v>
       </c>
       <c r="N13" s="33"/>
       <c r="O13" s="37" t="s">
+        <v>626</v>
+      </c>
+      <c r="P13" s="35" t="s">
+        <v>623</v>
+      </c>
+      <c r="Q13" s="40" t="s">
         <v>627</v>
-      </c>
-      <c r="P13" s="35" t="s">
-        <v>624</v>
-      </c>
-      <c r="Q13" s="40" t="s">
-        <v>628</v>
       </c>
       <c r="R13" s="38"/>
       <c r="S13" s="39"/>
     </row>
-    <row r="14" spans="1:19" s="7" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:19" s="7" customFormat="1" ht="46.8" x14ac:dyDescent="0.4">
       <c r="A14" s="63"/>
       <c r="B14" s="59" t="s">
         <v>14</v>
@@ -7005,35 +7039,47 @@
       <c r="C14" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="69">
         <v>44937</v>
       </c>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34">
+      <c r="E14" s="69">
+        <v>44952</v>
+      </c>
+      <c r="F14" s="69">
+        <v>44952</v>
+      </c>
+      <c r="G14" s="69">
+        <v>44952</v>
+      </c>
+      <c r="H14" s="69">
         <v>44953</v>
       </c>
-      <c r="J14" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="K14" s="36"/>
-      <c r="L14" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="M14" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="N14" s="33"/>
-      <c r="O14" s="41" t="s">
+      <c r="I14" s="69">
+        <v>44953</v>
+      </c>
+      <c r="J14" s="70" t="s">
+        <v>638</v>
+      </c>
+      <c r="K14" s="71">
+        <v>1</v>
+      </c>
+      <c r="L14" s="70" t="s">
+        <v>639</v>
+      </c>
+      <c r="M14" s="70" t="s">
+        <v>210</v>
+      </c>
+      <c r="N14" s="68" t="s">
+        <v>4</v>
+      </c>
+      <c r="O14" s="72" t="s">
+        <v>640</v>
+      </c>
+      <c r="P14" s="35" t="s">
+        <v>623</v>
+      </c>
+      <c r="Q14" s="40" t="s">
         <v>622</v>
-      </c>
-      <c r="P14" s="35" t="s">
-        <v>624</v>
-      </c>
-      <c r="Q14" s="40" t="s">
-        <v>623</v>
       </c>
       <c r="R14" s="38"/>
       <c r="S14" s="39"/>
@@ -8290,7 +8336,7 @@
       <c r="P40" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="Q40" s="65" t="s">
+      <c r="Q40" s="64" t="s">
         <v>175</v>
       </c>
       <c r="R40" s="42"/>
@@ -8339,7 +8385,7 @@
       <c r="P41" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="Q41" s="66"/>
+      <c r="Q41" s="65"/>
       <c r="R41" s="43"/>
       <c r="S41" s="39"/>
     </row>
@@ -8386,7 +8432,7 @@
       <c r="P42" s="35" t="s">
         <v>327</v>
       </c>
-      <c r="Q42" s="67"/>
+      <c r="Q42" s="66"/>
       <c r="R42" s="44"/>
       <c r="S42" s="39"/>
     </row>
@@ -8616,7 +8662,7 @@
         <v>556</v>
       </c>
       <c r="O47" s="41" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="P47" s="35" t="s">
         <v>547</v>
@@ -9009,16 +9055,16 @@
         <v>123</v>
       </c>
       <c r="N55" s="33" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="O55" s="41" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="P55" s="35" t="s">
         <v>621</v>
       </c>
       <c r="Q55" s="46" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="R55" s="40"/>
       <c r="S55" s="47"/>
@@ -9789,7 +9835,7 @@
       <c r="P71" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="Q71" s="65" t="s">
+      <c r="Q71" s="64" t="s">
         <v>258</v>
       </c>
       <c r="R71" s="42"/>
@@ -9838,7 +9884,7 @@
       <c r="P72" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="Q72" s="66"/>
+      <c r="Q72" s="65"/>
       <c r="R72" s="43"/>
       <c r="S72" s="39"/>
     </row>
@@ -9885,7 +9931,7 @@
       <c r="P73" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="Q73" s="66"/>
+      <c r="Q73" s="65"/>
       <c r="R73" s="43"/>
       <c r="S73" s="39"/>
     </row>
@@ -9932,7 +9978,7 @@
       <c r="P74" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="Q74" s="66"/>
+      <c r="Q74" s="65"/>
       <c r="R74" s="43"/>
       <c r="S74" s="39"/>
     </row>
@@ -9979,7 +10025,7 @@
       <c r="P75" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="Q75" s="66"/>
+      <c r="Q75" s="65"/>
       <c r="R75" s="43"/>
       <c r="S75" s="39"/>
     </row>
@@ -10026,7 +10072,7 @@
       <c r="P76" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="Q76" s="66"/>
+      <c r="Q76" s="65"/>
       <c r="R76" s="43"/>
       <c r="S76" s="39"/>
     </row>
@@ -10073,7 +10119,7 @@
       <c r="P77" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="Q77" s="66"/>
+      <c r="Q77" s="65"/>
       <c r="R77" s="43"/>
       <c r="S77" s="39"/>
     </row>
@@ -10120,7 +10166,7 @@
       <c r="P78" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="Q78" s="66"/>
+      <c r="Q78" s="65"/>
       <c r="R78" s="43"/>
       <c r="S78" s="39"/>
     </row>
@@ -10167,7 +10213,7 @@
       <c r="P79" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="Q79" s="67"/>
+      <c r="Q79" s="66"/>
       <c r="R79" s="44"/>
       <c r="S79" s="39"/>
     </row>
@@ -10257,7 +10303,7 @@
       <c r="P81" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="Q81" s="65" t="s">
+      <c r="Q81" s="64" t="s">
         <v>298</v>
       </c>
       <c r="R81" s="43"/>
@@ -10306,7 +10352,7 @@
       <c r="P82" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="Q82" s="66"/>
+      <c r="Q82" s="65"/>
       <c r="R82" s="43"/>
       <c r="S82" s="39"/>
     </row>
@@ -10353,7 +10399,7 @@
       <c r="P83" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="Q83" s="66"/>
+      <c r="Q83" s="65"/>
       <c r="R83" s="43"/>
       <c r="S83" s="39"/>
     </row>
@@ -10400,7 +10446,7 @@
       <c r="P84" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="Q84" s="66"/>
+      <c r="Q84" s="65"/>
       <c r="R84" s="43"/>
       <c r="S84" s="39"/>
     </row>
@@ -10447,7 +10493,7 @@
       <c r="P85" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="Q85" s="66"/>
+      <c r="Q85" s="65"/>
       <c r="R85" s="43"/>
       <c r="S85" s="39"/>
     </row>
@@ -10494,7 +10540,7 @@
       <c r="P86" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="Q86" s="66"/>
+      <c r="Q86" s="65"/>
       <c r="R86" s="43"/>
       <c r="S86" s="39"/>
     </row>
@@ -10535,7 +10581,7 @@
       <c r="P87" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="Q87" s="66"/>
+      <c r="Q87" s="65"/>
       <c r="R87" s="43"/>
       <c r="S87" s="39"/>
     </row>
@@ -10582,7 +10628,7 @@
       <c r="P88" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="Q88" s="66"/>
+      <c r="Q88" s="65"/>
       <c r="R88" s="43"/>
       <c r="S88" s="39"/>
     </row>
@@ -10629,7 +10675,7 @@
       <c r="P89" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="Q89" s="66"/>
+      <c r="Q89" s="65"/>
       <c r="R89" s="43"/>
       <c r="S89" s="39"/>
     </row>
@@ -10676,7 +10722,7 @@
       <c r="P90" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="Q90" s="67"/>
+      <c r="Q90" s="66"/>
       <c r="R90" s="43"/>
       <c r="S90" s="39"/>
     </row>
@@ -12169,7 +12215,7 @@
       <c r="P121" s="35" t="s">
         <v>191</v>
       </c>
-      <c r="Q121" s="65" t="s">
+      <c r="Q121" s="64" t="s">
         <v>200</v>
       </c>
       <c r="R121" s="42"/>
@@ -12218,7 +12264,7 @@
       <c r="P122" s="35" t="s">
         <v>196</v>
       </c>
-      <c r="Q122" s="67"/>
+      <c r="Q122" s="66"/>
       <c r="R122" s="44"/>
       <c r="S122" s="39"/>
     </row>
@@ -12522,7 +12568,7 @@
         <v>16</v>
       </c>
       <c r="C129" s="58" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D129" s="34">
         <v>44924</v>
@@ -12555,16 +12601,16 @@
         <v>25</v>
       </c>
       <c r="N129" s="33" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="O129" s="41" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="P129" s="35" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="Q129" s="46" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="R129" s="53"/>
       <c r="S129" s="39"/>
@@ -12898,7 +12944,7 @@
       <c r="P136" s="35" t="s">
         <v>327</v>
       </c>
-      <c r="Q136" s="65" t="s">
+      <c r="Q136" s="64" t="s">
         <v>263</v>
       </c>
       <c r="R136" s="40"/>
@@ -12947,7 +12993,7 @@
       <c r="P137" s="35" t="s">
         <v>327</v>
       </c>
-      <c r="Q137" s="66"/>
+      <c r="Q137" s="65"/>
       <c r="R137" s="40"/>
       <c r="S137" s="39"/>
     </row>
@@ -12994,7 +13040,7 @@
       <c r="P138" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="Q138" s="66"/>
+      <c r="Q138" s="65"/>
       <c r="R138" s="40"/>
       <c r="S138" s="39"/>
     </row>
@@ -13041,7 +13087,7 @@
       <c r="P139" s="35" t="s">
         <v>327</v>
       </c>
-      <c r="Q139" s="67"/>
+      <c r="Q139" s="66"/>
       <c r="R139" s="40"/>
       <c r="S139" s="39"/>
     </row>
@@ -15717,7 +15763,7 @@
       <c r="S194" s="39"/>
     </row>
     <row r="195" spans="1:19" s="7" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A195" s="64"/>
+      <c r="A195" s="67"/>
       <c r="B195" s="59" t="s">
         <v>21</v>
       </c>
@@ -15759,7 +15805,7 @@
       <c r="P195" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="Q195" s="65" t="s">
+      <c r="Q195" s="64" t="s">
         <v>176</v>
       </c>
       <c r="R195" s="42"/>
@@ -15808,7 +15854,7 @@
       <c r="P196" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="Q196" s="66"/>
+      <c r="Q196" s="65"/>
       <c r="R196" s="43"/>
       <c r="S196" s="39"/>
     </row>
@@ -15855,7 +15901,7 @@
       <c r="P197" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="Q197" s="66"/>
+      <c r="Q197" s="65"/>
       <c r="R197" s="43"/>
       <c r="S197" s="39"/>
     </row>
@@ -15902,7 +15948,7 @@
       <c r="P198" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="Q198" s="67"/>
+      <c r="Q198" s="66"/>
       <c r="R198" s="44"/>
       <c r="S198" s="39"/>
     </row>
@@ -15949,7 +15995,7 @@
       <c r="P199" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="Q199" s="65" t="s">
+      <c r="Q199" s="64" t="s">
         <v>177</v>
       </c>
       <c r="R199" s="42"/>
@@ -15998,7 +16044,7 @@
       <c r="P200" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="Q200" s="66"/>
+      <c r="Q200" s="65"/>
       <c r="R200" s="43"/>
       <c r="S200" s="39"/>
     </row>
@@ -16045,7 +16091,7 @@
       <c r="P201" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="Q201" s="66"/>
+      <c r="Q201" s="65"/>
       <c r="R201" s="43"/>
       <c r="S201" s="39"/>
     </row>
@@ -16092,7 +16138,7 @@
       <c r="P202" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="Q202" s="66"/>
+      <c r="Q202" s="65"/>
       <c r="R202" s="43"/>
       <c r="S202" s="39"/>
     </row>
@@ -16139,7 +16185,7 @@
       <c r="P203" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="Q203" s="67"/>
+      <c r="Q203" s="66"/>
       <c r="R203" s="44"/>
       <c r="S203" s="39"/>
     </row>
@@ -16830,6 +16876,11 @@
   </sheetData>
   <autoFilter ref="A6:Q217"/>
   <mergeCells count="15">
+    <mergeCell ref="A211:A217"/>
+    <mergeCell ref="A182:A183"/>
+    <mergeCell ref="A185:A195"/>
+    <mergeCell ref="A179:A181"/>
+    <mergeCell ref="A130:A178"/>
     <mergeCell ref="A7:A55"/>
     <mergeCell ref="A68:A129"/>
     <mergeCell ref="A56:A67"/>
@@ -16840,11 +16891,6 @@
     <mergeCell ref="Q136:Q139"/>
     <mergeCell ref="Q71:Q79"/>
     <mergeCell ref="Q81:Q90"/>
-    <mergeCell ref="A211:A217"/>
-    <mergeCell ref="A182:A183"/>
-    <mergeCell ref="A185:A195"/>
-    <mergeCell ref="A179:A181"/>
-    <mergeCell ref="A130:A178"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="D40:G48 D195:G200 D202:G210 J195:O200 D201:O201 D160:E160 D158:M159 N158:O160 J202:O210 D161:O168 D65:G66 D118:G118 D150:O157 D149:G149 D170:O170 D169:G169 D171:G176 D215:G215 J65:O66 J118:O118 J149:O149 J169:O169 J171:O176 J215:O215 J39:O48 H205:I210 J160:M160 D7:O38 D211:O214 D177:O194 D119:O148 D67:O117 D49:O64 D216:O1048576">

</xml_diff>